<commit_message>
just for practicing preprocessing data
</commit_message>
<xml_diff>
--- a/score.xlsx
+++ b/score.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26430" windowHeight="11115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26430" windowHeight="11120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,87 +26,87 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
   <si>
+    <t>언어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시각</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김김김</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>느느느</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마마마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보보보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>응응응</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장장장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추추추</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트트트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하하하</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ㄱ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀린</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀린</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ㄴ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>언어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시각</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>교재</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김김김</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>느느느</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마마마</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>보보보</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>응응응</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장장장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추추추</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>트트트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>하하하</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ㄱ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>틀린</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>total</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>틀린</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>total</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ㄴ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -158,10 +158,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,69 +446,68 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -535,12 +534,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -567,12 +566,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -599,12 +598,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -631,12 +630,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -663,12 +662,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -695,12 +694,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -727,9 +726,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -759,12 +758,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -791,12 +790,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -823,12 +822,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>7</v>
@@ -855,12 +854,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -887,12 +886,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -919,12 +918,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -951,12 +950,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>8</v>
@@ -983,12 +982,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>9</v>
@@ -1014,21 +1013,20 @@
       <c r="J18">
         <v>11</v>
       </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="L18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>11</v>
@@ -1055,12 +1053,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -1088,13 +1086,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
+  <mergeCells count="4">
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>